<commit_message>
Added many debugging print statements Added EOD stop orders including exchange specific EOD times Made the price change detection more versatile
</commit_message>
<xml_diff>
--- a/Shared Files/CompanyTickers.xlsx
+++ b/Shared Files/CompanyTickers.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3468" uniqueCount="2721">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3474" uniqueCount="2721">
   <si>
     <t>888 Holdings</t>
   </si>
@@ -19668,10 +19668,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19698,7 +19698,7 @@
         <v>10</v>
       </c>
       <c r="C2">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -19709,7 +19709,7 @@
         <v>50</v>
       </c>
       <c r="C3">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -19720,7 +19720,7 @@
         <v>100</v>
       </c>
       <c r="C4">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -19731,7 +19731,7 @@
         <v>500</v>
       </c>
       <c r="C5">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -19742,7 +19742,7 @@
         <v>1000</v>
       </c>
       <c r="C6">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -19753,7 +19753,7 @@
         <v>5000</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -20308,21 +20308,21 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>2698</v>
+        <v>2689</v>
       </c>
       <c r="B58">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C58">
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>2698</v>
+        <v>2689</v>
       </c>
       <c r="B59">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C59">
         <v>5.0000000000000001E-3</v>
@@ -20330,10 +20330,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>2698</v>
+        <v>2689</v>
       </c>
       <c r="B60">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C60">
         <v>0.01</v>
@@ -20341,12 +20341,78 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>2698</v>
+        <v>2689</v>
       </c>
       <c r="B61">
+        <v>50</v>
+      </c>
+      <c r="C61">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>2689</v>
+      </c>
+      <c r="B62">
         <v>100</v>
       </c>
-      <c r="C61">
+      <c r="C62">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>2689</v>
+      </c>
+      <c r="B63">
+        <v>500</v>
+      </c>
+      <c r="C63">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>2698</v>
+      </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
+      <c r="C64">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>2698</v>
+      </c>
+      <c r="B65">
+        <v>10</v>
+      </c>
+      <c r="C65">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>2698</v>
+      </c>
+      <c r="B66">
+        <v>50</v>
+      </c>
+      <c r="C66">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>2698</v>
+      </c>
+      <c r="B67">
+        <v>100</v>
+      </c>
+      <c r="C67">
         <v>0.05</v>
       </c>
     </row>

</xml_diff>